<commit_message>
Completed MOSCOW and Risk Assessment
</commit_message>
<xml_diff>
--- a/Documentation/Risk Assessment.xlsx
+++ b/Documentation/Risk Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QA\Desktop\IMS\IMS-22EnableMay2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15C8CBEF-78F3-4667-A5B0-F7A080E6EA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5E0176-E36C-4156-BEE0-ABC736EB7789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7FDBD9BC-9C30-4BBF-83F1-F1573D2F17F5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{7FDBD9BC-9C30-4BBF-83F1-F1573D2F17F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,10 +222,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -297,7 +311,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -331,58 +345,123 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -700,22 +779,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87F0CF8-F88A-4D21-ACF1-D6F81608C049}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.53125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.9296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.19921875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.9296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="9.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.46484375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.9296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.9296875" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.3984375" customWidth="1"/>
     <col min="12" max="12" width="13.59765625" customWidth="1"/>
     <col min="13" max="13" width="11.73046875" customWidth="1"/>
@@ -724,383 +803,405 @@
     <col min="16" max="16" width="11.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:17" ht="42.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="46.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="46.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="58.15" x14ac:dyDescent="0.45">
+      <c r="A6" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.45">
+      <c r="A8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="23.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="D16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="16" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" ht="57" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="F19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:D9">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>